<commit_message>
Got the Lua firmware onto the ESP32 but it did not include the math library so switched back to Adruino and ported the basic humidity functions to it.  Moved the Lua source to deprecated since will not be using.
</commit_message>
<xml_diff>
--- a/documentation/AbsoluteHumidityCalc.xlsx
+++ b/documentation/AbsoluteHumidityCalc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jsoft\elevation-mapping\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jsoft\workshop-drier\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545AEE39-2470-4AF6-8DC8-373ED0A08F0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90985423-C4F4-4EBD-AEA6-C331C5430E8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="866" yWindow="77" windowWidth="19363" windowHeight="10809" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2520" windowWidth="13757" windowHeight="13663" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t xml:space="preserve">   Length Foot</t>
   </si>
   <si>
-    <t>Pounds per Cubic Meter</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Width foot</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t xml:space="preserve">  Height foot</t>
   </si>
   <si>
-    <t>Pounds Per Cubic Foot</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Cubic Foot</t>
   </si>
   <si>
@@ -114,9 +108,6 @@
     <t>max pounds water contained in Desicant</t>
   </si>
   <si>
-    <t>Ounces per Cubic Foot</t>
-  </si>
-  <si>
     <t>If we take 80* RH air and dry it to 10% then allow them to mix then</t>
   </si>
   <si>
@@ -172,6 +163,15 @@
   </si>
   <si>
     <t xml:space="preserve">for example: If low temp will be 40F or 4.4C  the air can hold 6.6 grams at 100%  vs our 12 grams. </t>
+  </si>
+  <si>
+    <t>grams per ounce</t>
+  </si>
+  <si>
+    <t>ounces per  cubic foot</t>
+  </si>
+  <si>
+    <t>pounds per cubic foot</t>
   </si>
 </sst>
 </file>
@@ -183,9 +183,9 @@
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0.0000000"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="172" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -259,6 +259,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -278,11 +284,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -303,7 +310,7 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -313,8 +320,10 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -534,8 +543,8 @@
   </sheetPr>
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -551,10 +560,10 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -564,7 +573,7 @@
       </c>
       <c r="B3" s="15">
         <f>(B2-32)/1.8</f>
-        <v>4.4444444444444446</v>
+        <v>21.111111111111111</v>
       </c>
       <c r="C3" s="3"/>
     </row>
@@ -573,7 +582,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4">
-        <v>99.998999999999995</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -581,13 +590,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="12.9" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="7">
         <f>(6.112 * POWER(2.71828,((17.67 * B3)/(B3 + 243.5))) * B4 * 2.1674) / (273.15 + B3)</f>
-        <v>6.5503515637723142</v>
+        <v>14.747628408008804</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>5</v>
@@ -596,61 +605,60 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="12.9" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="8">
+        <v>28.349499999999999</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>6</v>
-      </c>
-      <c r="B7" s="8">
-        <f>B6/453.92</f>
-        <v>1.4430629987161424E-2</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>7</v>
       </c>
       <c r="G7" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="12.9" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="6">
         <v>35.314700000000002</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="12.9" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B9" s="10">
-        <f>B7/B8</f>
-        <v>4.0862955050337176E-4</v>
+        <f>(B6/B7)/B8</f>
+        <v>1.4730627972189355E-2</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G9" s="11">
         <f>G8*G7*G6</f>
         <v>22464</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="12.9" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" s="12">
         <f>B6/1000</f>
-        <v>6.5503515637723138E-3</v>
+        <v>1.4747628408008804E-2</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G10" s="11">
         <f>G9/35.3147</f>
@@ -659,36 +667,36 @@
     </row>
     <row r="11" spans="1:7" ht="12.9" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B11" s="20">
-        <f>B7*16</f>
-        <v>0.23089007979458279</v>
+        <f>B9/16</f>
+        <v>9.2066424826183467E-4</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G11" s="11">
         <f>G10*B6</f>
-        <v>4166.7378606807151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>9381.0997844384838</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="12.9" x14ac:dyDescent="0.35">
       <c r="F12" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G12" s="11">
         <f>G11/453.592</f>
-        <v>9.1860920401610162</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20.681801672953853</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="12.9" x14ac:dyDescent="0.35">
       <c r="F13" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G13" s="11">
         <f>G11/3785.41</f>
-        <v>1.1007362110526244</v>
+        <v>2.4782255513771254</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -698,32 +706,36 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="str">
+      <c r="A15" s="26" t="str">
         <f>HYPERLINK("https://www.process-heating.com/ext/resources/PH/2001/05/Files/PDFs/0501PHhartzell-tables1and2.pdf","Process Heating Chart")</f>
         <v>Process Heating Chart</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F16" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F17" s="16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F18" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
+      <c r="B19">
+        <f>2.2/6.8</f>
+        <v>0.3235294117647059</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G20">
         <v>6</v>
@@ -735,33 +747,37 @@
         <v>1001.1539593804506</v>
       </c>
       <c r="F21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G21" s="18">
         <v>0.15</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <f>3.68*0.53</f>
+        <v>1.9504000000000001</v>
+      </c>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G22">
         <f>G12/G21</f>
-        <v>61.240613601073441</v>
+        <v>137.87867781969237</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G23">
         <f>G22/G20</f>
-        <v>10.20676893351224</v>
+        <v>22.979779636615394</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G24" s="19">
         <v>0.4</v>
@@ -769,20 +785,20 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G25">
         <f>G23/G24</f>
-        <v>25.516922333780599</v>
+        <v>57.449449091538483</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G26">
         <f>G25*G21</f>
-        <v>3.8275383500670896</v>
+        <v>8.6174173637307714</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -790,12 +806,12 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F30" s="25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F31" s="21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G31">
         <v>12.12</v>
@@ -807,79 +823,85 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F32" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F33" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F38" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F39" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F40" s="21"/>
+    </row>
+    <row r="41" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F41" s="21"/>
+    </row>
+    <row r="42" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F42" s="21"/>
+    </row>
+    <row r="43" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F43" s="24" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F33" s="21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F35" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F36" s="21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F37" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F38" s="21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F39" s="21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F40" s="21"/>
-    </row>
-    <row r="41" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F41" s="21"/>
-    </row>
-    <row r="42" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F42" s="21"/>
-    </row>
-    <row r="43" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F43" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F44" s="21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F45" s="21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E46" s="26" t="str">
+        <f>HYPERLINK("https://www.process-heating.com/ext/resources/PH/2001/05/Files/PDFs/0501PHhartzell-tables1and2.pdf","Process Heating Chart")</f>
+        <v>Process Heating Chart</v>
+      </c>
+    </row>
+    <row r="47" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F47" s="21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G47">
         <v>10.606</v>
       </c>
     </row>
-    <row r="48" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F48" s="21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G48">
         <v>1.3260000000000001</v>
@@ -887,7 +909,7 @@
     </row>
     <row r="49" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F49" s="21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G49">
         <v>5.9660000000000002</v>
@@ -895,15 +917,15 @@
     </row>
     <row r="50" spans="6:8" ht="42.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G50" s="23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H50" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F51" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G51" s="22">
         <f>(G$47+(G$48*H51))/(H51+1)</f>
@@ -915,7 +937,7 @@
     </row>
     <row r="52" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F52" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G52" s="22">
         <f t="shared" ref="G52:G69" si="0">(G$47+(G$48*H52))/(H52+1)</f>
@@ -927,7 +949,7 @@
     </row>
     <row r="53" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F53" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G53" s="22">
         <f t="shared" si="0"/>
@@ -939,7 +961,7 @@
     </row>
     <row r="54" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F54" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G54" s="22">
         <f t="shared" si="0"/>
@@ -951,7 +973,7 @@
     </row>
     <row r="55" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F55" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G55" s="22">
         <f t="shared" si="0"/>
@@ -963,7 +985,7 @@
     </row>
     <row r="56" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F56" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G56" s="22">
         <f t="shared" si="0"/>
@@ -975,7 +997,7 @@
     </row>
     <row r="57" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F57" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G57" s="22">
         <f t="shared" si="0"/>
@@ -987,7 +1009,7 @@
     </row>
     <row r="58" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F58" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G58" s="22">
         <f t="shared" si="0"/>
@@ -999,7 +1021,7 @@
     </row>
     <row r="59" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F59" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G59" s="22">
         <f t="shared" si="0"/>
@@ -1011,7 +1033,7 @@
     </row>
     <row r="60" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F60" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G60" s="22">
         <f t="shared" si="0"/>
@@ -1023,7 +1045,7 @@
     </row>
     <row r="61" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F61" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G61" s="22">
         <f t="shared" si="0"/>
@@ -1035,7 +1057,7 @@
     </row>
     <row r="62" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F62" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G62" s="22">
         <f t="shared" si="0"/>
@@ -1047,7 +1069,7 @@
     </row>
     <row r="63" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F63" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G63" s="22">
         <f t="shared" si="0"/>
@@ -1059,7 +1081,7 @@
     </row>
     <row r="64" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F64" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G64" s="22">
         <f t="shared" si="0"/>
@@ -1071,7 +1093,7 @@
     </row>
     <row r="65" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F65" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G65" s="22">
         <f t="shared" si="0"/>
@@ -1083,7 +1105,7 @@
     </row>
     <row r="66" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F66" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G66" s="22">
         <f t="shared" si="0"/>
@@ -1095,7 +1117,7 @@
     </row>
     <row r="67" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F67" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G67" s="22">
         <f t="shared" si="0"/>
@@ -1107,7 +1129,7 @@
     </row>
     <row r="68" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F68" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G68" s="22">
         <f t="shared" si="0"/>
@@ -1119,7 +1141,7 @@
     </row>
     <row r="69" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F69" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G69" s="22">
         <f t="shared" si="0"/>

</xml_diff>